<commit_message>
[Feat 2269] Addded support of parameters worksheet metadata Replaced steps related  string litterals in export with the matching enum
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
     <sheet name="STEPS" sheetId="2" r:id="rId2"/>
-    <sheet name="PARAMETERS TODO" sheetId="3" r:id="rId3"/>
+    <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS TODO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>ACTION</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>TC_STEP_EXPECTED_RESULT</t>
+  </si>
+  <si>
+    <t>TC_PARAM_ID</t>
+  </si>
+  <si>
+    <t>TC_PARAM_NAME</t>
+  </si>
+  <si>
+    <t>TC_PARAM_DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1170,12 +1179,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[Feat 2269] Addded support of datasets worksheet metadata Replaced steps related  string litterals in export with the matching enum
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
     <sheet name="STEPS" sheetId="2" r:id="rId2"/>
     <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
-    <sheet name="DATASETS TODO" sheetId="4" r:id="rId4"/>
+    <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>ACTION</t>
   </si>
@@ -155,6 +155,24 @@
   </si>
   <si>
     <t>TC_PARAM_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>TC_DATASET_ID</t>
+  </si>
+  <si>
+    <t>TC_DATASET_NAME</t>
+  </si>
+  <si>
+    <t>TC_PARAM_OWNER_ID</t>
+  </si>
+  <si>
+    <t>TC_DATASET_PARAM_VALUE</t>
+  </si>
+  <si>
+    <t>TC_DATASET_PARAM_NAME</t>
+  </si>
+  <si>
+    <t>TC_PARAM_OWNER_PATH</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1221,12 +1239,54 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Feat 2269] Addded support of steps worksheet metadata Replaced steps related  string litterals in export with the matching enum
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
-    <sheet name="STEPS TODO" sheetId="2" r:id="rId2"/>
+    <sheet name="STEPS" sheetId="2" r:id="rId2"/>
     <sheet name="PARAMETERS TODO" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS TODO" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>ACTION</t>
   </si>
@@ -116,6 +116,36 @@
   </si>
   <si>
     <t>TC_#_CALLED_BY</t>
+  </si>
+  <si>
+    <t>TC_STEP_ID</t>
+  </si>
+  <si>
+    <t>TC_STEP_NUM</t>
+  </si>
+  <si>
+    <t>TC_STEP_ACTION</t>
+  </si>
+  <si>
+    <t>TC_STEP_#_REQ</t>
+  </si>
+  <si>
+    <t>TC_STEP_#_ATTACHMENT</t>
+  </si>
+  <si>
+    <t>TC_STEP_CUF_&lt;CODE&gt;</t>
+  </si>
+  <si>
+    <t>TC_OWNER_PATH</t>
+  </si>
+  <si>
+    <t>TC_OWNER_ID</t>
+  </si>
+  <si>
+    <t>TC_STEP_IS_CALL_STEP</t>
+  </si>
+  <si>
+    <t>TC_STEP_EXPECTED_RESULT</t>
   </si>
 </sst>
 </file>
@@ -557,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
@@ -1077,12 +1107,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
[Feat 2269][Feat 3238] Parser reads the test case worksheet and creates TestCaseInstructions accordingly. Custom field are not yet processed Error cases are not yet handled : when a cell is not parsable, process throws an  exception
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>ACTION</t>
   </si>
@@ -173,6 +173,36 @@
   </si>
   <si>
     <t>TC_PARAM_OWNER_PATH</t>
+  </si>
+  <si>
+    <t>path/row1</t>
+  </si>
+  <si>
+    <t>path/row2</t>
+  </si>
+  <si>
+    <t>path/row4</t>
+  </si>
+  <si>
+    <t>path/row5</t>
+  </si>
+  <si>
+    <t>path/row6</t>
+  </si>
+  <si>
+    <t>path/row7</t>
+  </si>
+  <si>
+    <t>path/row8</t>
+  </si>
+  <si>
+    <t>path/row9</t>
+  </si>
+  <si>
+    <t>path/row10</t>
+  </si>
+  <si>
+    <t>path/row3</t>
   </si>
 </sst>
 </file>
@@ -612,17 +642,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
@@ -724,8 +754,12 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3">
+        <v>11</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -752,8 +786,12 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -780,8 +818,12 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3">
+        <v>13</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -808,8 +850,12 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="3">
+        <v>14</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -836,8 +882,12 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="3">
+        <v>15</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -864,8 +914,12 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="3">
+        <v>16</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -892,8 +946,12 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="3">
+        <v>17</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -920,8 +978,12 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="3">
+        <v>18</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
@@ -946,8 +1008,12 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="3">
+        <v>19</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -974,8 +1040,12 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="D11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="3">
+        <v>20</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -996,136 +1066,6 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1137,7 +1077,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Feat 2269][Feat 3238] Fixed : parser only processed mandatory columns
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>ACTION</t>
   </si>
@@ -203,6 +203,66 @@
   </si>
   <si>
     <t>path/row3</t>
+  </si>
+  <si>
+    <t>ref1</t>
+  </si>
+  <si>
+    <t>ref2</t>
+  </si>
+  <si>
+    <t>ref3</t>
+  </si>
+  <si>
+    <t>ref4</t>
+  </si>
+  <si>
+    <t>ref5</t>
+  </si>
+  <si>
+    <t>ref6</t>
+  </si>
+  <si>
+    <t>ref7</t>
+  </si>
+  <si>
+    <t>ref8</t>
+  </si>
+  <si>
+    <t>ref9</t>
+  </si>
+  <si>
+    <t>ref10</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>name4</t>
+  </si>
+  <si>
+    <t>name5</t>
+  </si>
+  <si>
+    <t>name6</t>
+  </si>
+  <si>
+    <t>name7</t>
+  </si>
+  <si>
+    <t>name8</t>
+  </si>
+  <si>
+    <t>name9</t>
+  </si>
+  <si>
+    <t>name10</t>
   </si>
 </sst>
 </file>
@@ -645,7 +705,7 @@
   <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,8 +821,12 @@
         <v>11</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -793,8 +857,12 @@
         <v>12</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -825,8 +893,12 @@
         <v>13</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -857,8 +929,12 @@
         <v>14</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -889,8 +965,12 @@
         <v>15</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -921,8 +1001,12 @@
         <v>16</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -953,8 +1037,12 @@
         <v>17</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="G8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -985,8 +1073,12 @@
         <v>18</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -1015,8 +1107,12 @@
         <v>19</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="G10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1047,8 +1143,12 @@
         <v>20</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1077,7 +1177,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[Feat 2269][Feat 3238] Added custom coercer for ImportMode enum cells which follow special rules. Coertion exceptions are swallowed (logged) to that they don't break the parser's  unit tests. Must still be properly handled.
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
   <si>
     <t>ACTION</t>
   </si>
@@ -94,12 +94,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>REPLACE</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>UPDATE</t>
   </si>
   <si>
@@ -196,12 +190,6 @@
     <t>path/row8</t>
   </si>
   <si>
-    <t>path/row9</t>
-  </si>
-  <si>
-    <t>path/row10</t>
-  </si>
-  <si>
     <t>path/row3</t>
   </si>
   <si>
@@ -229,12 +217,6 @@
     <t>ref8</t>
   </si>
   <si>
-    <t>ref9</t>
-  </si>
-  <si>
-    <t>ref10</t>
-  </si>
-  <si>
     <t>name1</t>
   </si>
   <si>
@@ -259,10 +241,76 @@
     <t>name8</t>
   </si>
   <si>
-    <t>name9</t>
-  </si>
-  <si>
-    <t>name10</t>
+    <t>desc1</t>
+  </si>
+  <si>
+    <t>desc2</t>
+  </si>
+  <si>
+    <t>desc3</t>
+  </si>
+  <si>
+    <t>desc4</t>
+  </si>
+  <si>
+    <t>desc5</t>
+  </si>
+  <si>
+    <t>desc6</t>
+  </si>
+  <si>
+    <t>desc7</t>
+  </si>
+  <si>
+    <t>desc8</t>
+  </si>
+  <si>
+    <t>pre1</t>
+  </si>
+  <si>
+    <t>pre2</t>
+  </si>
+  <si>
+    <t>pre3</t>
+  </si>
+  <si>
+    <t>pre4</t>
+  </si>
+  <si>
+    <t>pre5</t>
+  </si>
+  <si>
+    <t>pre6</t>
+  </si>
+  <si>
+    <t>pre7</t>
+  </si>
+  <si>
+    <t>pre8</t>
+  </si>
+  <si>
+    <t>creator1</t>
+  </si>
+  <si>
+    <t>creator2</t>
+  </si>
+  <si>
+    <t>creator3</t>
+  </si>
+  <si>
+    <t>creator4</t>
+  </si>
+  <si>
+    <t>creator5</t>
+  </si>
+  <si>
+    <t>creator6</t>
+  </si>
+  <si>
+    <t>creator7</t>
+  </si>
+  <si>
+    <t>creator8</t>
   </si>
 </sst>
 </file>
@@ -392,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -401,6 +449,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +833,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>16</v>
@@ -815,30 +864,38 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="3">
         <v>11</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="S2" s="8">
+        <v>37653</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
@@ -851,30 +908,38 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3">
         <v>12</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="N3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
+      <c r="S3" s="8">
+        <v>37654</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -887,30 +952,38 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3">
         <v>13</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="N4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="S4" s="8">
+        <v>37655</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
@@ -923,30 +996,38 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="3">
         <v>14</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="N5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
+      <c r="S5" s="8">
+        <v>37656</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
@@ -959,212 +1040,172 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3">
         <v>15</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="N6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
+      <c r="S6" s="8">
+        <v>37657</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3">
         <v>16</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="8">
+        <v>37658</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3">
         <v>17</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="N8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="S8" s="8">
+        <v>37659</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3">
         <v>18</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="3">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="3">
-        <v>20</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
+      <c r="O9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="8">
+        <v>37660</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1200,34 +1241,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1257,19 +1298,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1302,28 +1343,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat 2269][Feat 3238] Added EWP tests for happy pathes, fixed NPE in EWP when workbook don't contain all the possible sheets
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
   <si>
     <t>ACTION</t>
   </si>
@@ -311,6 +311,153 @@
   </si>
   <si>
     <t>creator8</t>
+  </si>
+  <si>
+    <t>owner/path/1</t>
+  </si>
+  <si>
+    <t>owner/path/2</t>
+  </si>
+  <si>
+    <t>owner/path/3</t>
+  </si>
+  <si>
+    <t>owner/path/4</t>
+  </si>
+  <si>
+    <t>owner/path/5</t>
+  </si>
+  <si>
+    <t>owner/path/6</t>
+  </si>
+  <si>
+    <t>owner/path/7</t>
+  </si>
+  <si>
+    <t>owner/path/8</t>
+  </si>
+  <si>
+    <t>action1</t>
+  </si>
+  <si>
+    <t>action2</t>
+  </si>
+  <si>
+    <t>action3</t>
+  </si>
+  <si>
+    <t>action4</t>
+  </si>
+  <si>
+    <t>action5</t>
+  </si>
+  <si>
+    <t>action6</t>
+  </si>
+  <si>
+    <t>action7</t>
+  </si>
+  <si>
+    <t>action8</t>
+  </si>
+  <si>
+    <t>result1</t>
+  </si>
+  <si>
+    <t>result2</t>
+  </si>
+  <si>
+    <t>result3</t>
+  </si>
+  <si>
+    <t>result4</t>
+  </si>
+  <si>
+    <t>result5</t>
+  </si>
+  <si>
+    <t>result6</t>
+  </si>
+  <si>
+    <t>result7</t>
+  </si>
+  <si>
+    <t>result8</t>
+  </si>
+  <si>
+    <t>paramName1</t>
+  </si>
+  <si>
+    <t>paramName2</t>
+  </si>
+  <si>
+    <t>paramName3</t>
+  </si>
+  <si>
+    <t>paramName4</t>
+  </si>
+  <si>
+    <t>paramName5</t>
+  </si>
+  <si>
+    <t>paramName6</t>
+  </si>
+  <si>
+    <t>paramName7</t>
+  </si>
+  <si>
+    <t>paramName8</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>value3</t>
+  </si>
+  <si>
+    <t>value4</t>
+  </si>
+  <si>
+    <t>value5</t>
+  </si>
+  <si>
+    <t>value6</t>
+  </si>
+  <si>
+    <t>value7</t>
+  </si>
+  <si>
+    <t>value8</t>
+  </si>
+  <si>
+    <t>param/owner/path/1</t>
+  </si>
+  <si>
+    <t>param/owner/path/2</t>
+  </si>
+  <si>
+    <t>param/owner/path/3</t>
+  </si>
+  <si>
+    <t>param/owner/path/4</t>
+  </si>
+  <si>
+    <t>param/owner/path/5</t>
+  </si>
+  <si>
+    <t>param/owner/path/6</t>
+  </si>
+  <si>
+    <t>param/owner/path/7</t>
+  </si>
+  <si>
+    <t>param/owner/path/8</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -440,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -450,6 +597,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,9 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1215,10 +1362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,51 +1384,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>13</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,36 +1630,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,35 +1799,218 @@
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat 3695] mostly functionnal, but not out of the wood yet.
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21312" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="148">
   <si>
     <t>ACTION</t>
   </si>
@@ -458,13 +458,16 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>TC_STEP_CALL_DATASET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,7 +691,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -723,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,38 +900,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1048,7 +1049,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1093,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1137,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1180,7 +1181,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1225,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1269,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1310,7 +1311,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1361,29 +1362,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1403,22 +1405,25 @@
         <v>39</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1433,17 +1438,18 @@
       <c r="F2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1458,17 +1464,18 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1483,17 +1490,18 @@
       <c r="F4" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1506,17 +1514,18 @@
         <v>14</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1529,17 +1538,18 @@
         <v>15</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1552,17 +1562,18 @@
         <v>16</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1573,17 +1584,18 @@
         <v>17</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1596,15 +1608,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1613,23 +1626,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1665,7 +1678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1681,7 +1694,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1710,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1713,7 +1726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1729,7 +1742,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1759,7 +1772,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1782,27 +1795,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1854,7 +1867,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1877,7 +1890,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1900,7 +1913,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1923,7 +1936,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1959,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1969,7 +1982,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1990,7 +2003,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Merge with branch evol-3577-postgresql
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21312" windowHeight="12780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="148">
   <si>
     <t>ACTION</t>
   </si>
@@ -458,13 +458,16 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>TC_STEP_CALL_DATASET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -688,7 +691,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -723,7 +725,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -899,38 +900,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1048,7 +1049,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1092,7 +1093,7 @@
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1136,7 +1137,7 @@
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1180,7 +1181,7 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1225,7 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1269,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1310,7 +1311,7 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1361,29 +1362,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1403,22 +1405,25 @@
         <v>39</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1433,17 +1438,18 @@
       <c r="F2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1458,17 +1464,18 @@
       <c r="F3" s="2">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1483,17 +1490,18 @@
       <c r="F4" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1506,17 +1514,18 @@
         <v>14</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1529,17 +1538,18 @@
         <v>15</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1552,17 +1562,18 @@
         <v>16</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1573,17 +1584,18 @@
         <v>17</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1596,15 +1608,16 @@
         <v>18</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1613,23 +1626,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1665,7 +1678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1681,7 +1694,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1710,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1713,7 +1726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1729,7 +1742,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1759,7 +1772,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1782,27 +1795,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -1854,7 +1867,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1877,7 +1890,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1900,7 +1913,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1923,7 +1936,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1946,7 +1959,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -1969,7 +1982,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>104</v>
@@ -1990,7 +2003,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
[Feat 3627] Excel export TC and Requirements
</commit_message>
<xml_diff>
--- a/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
+++ b/tm/tm.service/src/test/resources/batchimport/testcase/import-2269.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="21312" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="21315" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="TEST_CASES" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="PARAMETERS" sheetId="3" r:id="rId3"/>
     <sheet name="DATASETS" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="149">
   <si>
     <t>ACTION</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>TC_STEP_CALL_DATASET</t>
+  </si>
+  <si>
+    <t>TC_MILESTONE</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -901,37 +904,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -957,55 +963,58 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1029,27 +1038,28 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
-      <c r="S2" s="8">
+      <c r="S2" s="3"/>
+      <c r="T2" s="8">
         <v>37653</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="3"/>
+    </row>
+    <row r="3" spans="1:25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1073,27 +1083,28 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2"/>
+      <c r="O3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="8">
+      <c r="S3" s="2"/>
+      <c r="T3" s="8">
         <v>37654</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="2"/>
+    </row>
+    <row r="4" spans="1:25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1112,32 +1123,33 @@
       <c r="H4" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2"/>
+      <c r="O4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="8">
+      <c r="S4" s="2"/>
+      <c r="T4" s="8">
         <v>37655</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="2"/>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1161,27 +1173,28 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2"/>
+      <c r="O5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="8">
+      <c r="S5" s="2"/>
+      <c r="T5" s="8">
         <v>37656</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="U5" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="Y5" s="2"/>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1200,32 +1213,33 @@
       <c r="H6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2"/>
+      <c r="O6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="8">
+      <c r="S6" s="2"/>
+      <c r="T6" s="8">
         <v>37657</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="U6" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" s="7" t="s">
         <v>28</v>
       </c>
@@ -1249,27 +1263,28 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="7"/>
+      <c r="O7" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="8">
+      <c r="S7" s="7"/>
+      <c r="T7" s="8">
         <v>37658</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7" s="7"/>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1286,32 +1301,33 @@
       <c r="H8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="2"/>
+      <c r="O8" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="8">
+      <c r="S8" s="2"/>
+      <c r="T8" s="8">
         <v>37659</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="U8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="U8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
@@ -1335,25 +1351,26 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="2"/>
+      <c r="O9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="8">
+      <c r="S9" s="2"/>
+      <c r="T9" s="8">
         <v>37660</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="U9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1365,24 +1382,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1633,13 +1650,13 @@
       <selection activeCell="E2" sqref="E2:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1802,17 +1819,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">

</xml_diff>